<commit_message>
made revisions to config.xlsx for the breadcrumb project
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rchristensen\repos\course-repos\optimal-estimation-course\06-course-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labuser\Desktop\breadcrumb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857E828A-E18E-4BE1-B9B6-670D3044F96A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D810ED-CAF2-4E77-82D7-E335A9D164B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="14400" windowHeight="8190" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="14400" windowHeight="8190" tabRatio="894" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="167">
   <si>
     <t>Value</t>
   </si>
@@ -122,9 +122,6 @@
     <t>del_gyrox</t>
   </si>
   <si>
-    <t>Injected gyro bias error</t>
-  </si>
-  <si>
     <t>del_gyroy</t>
   </si>
   <si>
@@ -137,15 +134,6 @@
     <t>Gyro bias ECRV time constant</t>
   </si>
   <si>
-    <t>pos</t>
-  </si>
-  <si>
-    <t>vel</t>
-  </si>
-  <si>
-    <t>att</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -182,129 +170,36 @@
     <t>tsim</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>MU</t>
-  </si>
-  <si>
     <t>corrRV</t>
   </si>
   <si>
-    <t>Orb_alt0</t>
-  </si>
-  <si>
-    <t>Orb_altf</t>
-  </si>
-  <si>
-    <t>R_M</t>
-  </si>
-  <si>
-    <t>R_EQ</t>
-  </si>
-  <si>
-    <t>lx</t>
-  </si>
-  <si>
-    <t>ly</t>
-  </si>
-  <si>
-    <t>lz</t>
-  </si>
-  <si>
-    <t>km^3/s^2</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>deg/day</t>
-  </si>
-  <si>
     <t>Simulation timestep</t>
   </si>
   <si>
     <t>Simulation time</t>
   </si>
   <si>
-    <t>Period of Orbit</t>
-  </si>
-  <si>
     <t>n_Qnoise</t>
   </si>
   <si>
     <t>number of Process noise componenets</t>
   </si>
   <si>
-    <t>gravity</t>
-  </si>
-  <si>
     <t>Correlatation of position and velocity</t>
   </si>
   <si>
-    <t>Initial Altitude of mapping orbit</t>
-  </si>
-  <si>
-    <t>Final Altitude of mapping orbit</t>
-  </si>
-  <si>
-    <t>Moon's mean radius</t>
-  </si>
-  <si>
-    <t>Moon's equatorial radius</t>
-  </si>
-  <si>
-    <t>Moon's rotational rate</t>
-  </si>
-  <si>
-    <t>x component of lever arm to TC (in body frame)</t>
-  </si>
-  <si>
-    <t>y component of lever arm to TC (in body frame)</t>
-  </si>
-  <si>
-    <t>z component of lever arm to TC (in body frame)</t>
-  </si>
-  <si>
-    <t>Star camera misalignment ECRV time constant</t>
-  </si>
-  <si>
-    <t>Terrain camera misalignment ECRV time constant</t>
-  </si>
-  <si>
-    <t>gbias</t>
-  </si>
-  <si>
-    <t>stmis</t>
-  </si>
-  <si>
-    <t>cmis</t>
-  </si>
-  <si>
     <t>ri_x</t>
   </si>
   <si>
-    <t>x component of initial position of spacecraft(inertial)</t>
-  </si>
-  <si>
     <t>ri_y</t>
   </si>
   <si>
-    <t>y component of initial position of spacecraft(inertial)</t>
-  </si>
-  <si>
     <t>ri_z</t>
   </si>
   <si>
-    <t>z component of initial position of spacecraft(inertial)</t>
-  </si>
-  <si>
     <t>vi_x</t>
   </si>
   <si>
-    <t>km/s</t>
-  </si>
-  <si>
     <t>vi_y</t>
   </si>
   <si>
@@ -416,99 +311,15 @@
     <t>sig_thstz</t>
   </si>
   <si>
-    <t>del_rsx</t>
-  </si>
-  <si>
-    <t>del_rsy</t>
-  </si>
-  <si>
-    <t>del_rsz</t>
-  </si>
-  <si>
-    <t>del_vsx</t>
-  </si>
-  <si>
-    <t>del_vsy</t>
-  </si>
-  <si>
-    <t>del_vsz</t>
-  </si>
-  <si>
-    <t>del_ax</t>
-  </si>
-  <si>
-    <t>del_ay</t>
-  </si>
-  <si>
-    <t>del_az</t>
-  </si>
-  <si>
-    <t>del_thstx</t>
-  </si>
-  <si>
-    <t>del_thsty</t>
-  </si>
-  <si>
-    <t>del_thstz</t>
-  </si>
-  <si>
-    <t>del_thcx</t>
-  </si>
-  <si>
-    <t>del_thcy</t>
-  </si>
-  <si>
-    <t>del_thcz</t>
-  </si>
-  <si>
-    <t>W_MOON</t>
-  </si>
-  <si>
     <t>MatlabValues</t>
   </si>
   <si>
-    <t>processStarTrackerEnable</t>
-  </si>
-  <si>
-    <t>processVisualOdometryEnable</t>
-  </si>
-  <si>
-    <t>tau_st</t>
-  </si>
-  <si>
-    <t>tau_c</t>
-  </si>
-  <si>
-    <t>Injected satellite position error</t>
-  </si>
-  <si>
-    <t>Injected satellite velocity error</t>
-  </si>
-  <si>
-    <t>Injected satellite orientation error</t>
-  </si>
-  <si>
-    <t>Injected star camera misalignment error</t>
-  </si>
-  <si>
-    <t>Injected terrain camera misalignment error</t>
-  </si>
-  <si>
     <t>th_z</t>
   </si>
   <si>
     <t>th_y</t>
   </si>
   <si>
-    <t>z angle of a ZYX euler angle sequence to define initial orientation of spacecraft</t>
-  </si>
-  <si>
-    <t>y angle of a ZYX euler angle sequence to define initial orientation of spacecraft</t>
-  </si>
-  <si>
-    <t>x angle of a ZYX euler angle sequence to define initial orientation of spacecraft</t>
-  </si>
-  <si>
     <t>th_x</t>
   </si>
   <si>
@@ -524,12 +335,6 @@
     <t>3-sigma non-gravitational process noise</t>
   </si>
   <si>
-    <t>flag to enable processing of star camera measurements</t>
-  </si>
-  <si>
-    <t>flag to enable processing of VO measurements</t>
-  </si>
-  <si>
     <t>pixels</t>
   </si>
   <si>
@@ -545,15 +350,6 @@
     <t>3-sigma u component of pixel noise</t>
   </si>
   <si>
-    <t>n_features</t>
-  </si>
-  <si>
-    <t>features</t>
-  </si>
-  <si>
-    <t>alpha</t>
-  </si>
-  <si>
     <t>thx_st</t>
   </si>
   <si>
@@ -611,67 +407,136 @@
     <t>days2hrs</t>
   </si>
   <si>
-    <t>focal_length</t>
-  </si>
-  <si>
-    <t>microns</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
-    <t>Hresolution</t>
-  </si>
-  <si>
-    <t>Vresolution</t>
-  </si>
-  <si>
-    <t>camera focal length</t>
-  </si>
-  <si>
-    <t>pixel pitch</t>
-  </si>
-  <si>
-    <t>horizontal resolution</t>
-  </si>
-  <si>
-    <t>vertical resolution</t>
-  </si>
-  <si>
-    <t>detector skewness</t>
-  </si>
-  <si>
-    <t>number of features to detect</t>
-  </si>
-  <si>
-    <t>pixel_pitch</t>
-  </si>
-  <si>
-    <t>vo_iterations</t>
-  </si>
-  <si>
-    <t>number of MLE iterations to refine the direction of motion estimate</t>
-  </si>
-  <si>
-    <t>flag to enable printing of VO diagnostic data</t>
-  </si>
-  <si>
-    <t>vo_diagnostics_enable</t>
-  </si>
-  <si>
-    <t>mrad</t>
-  </si>
-  <si>
-    <t>use_approx_cam_attitude_change_enable</t>
-  </si>
-  <si>
-    <t>flag to enable approximate modeling or moon-referenced camera attitude change</t>
-  </si>
-  <si>
     <t>correlated_kalman_update_enable</t>
   </si>
   <si>
     <t>flag to enable correlated Kalman update</t>
+  </si>
+  <si>
+    <t>position of antennas in body frame</t>
+  </si>
+  <si>
+    <t>distance between antennas</t>
+  </si>
+  <si>
+    <t>orientation of antennas</t>
+  </si>
+  <si>
+    <t>height of antennas above rfid tags</t>
+  </si>
+  <si>
+    <t>x component of initial position of vehicle (inertial)</t>
+  </si>
+  <si>
+    <t>y component of initial position of vehicle (inertial)</t>
+  </si>
+  <si>
+    <t>z component of initial position of vehicle (inertial)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z angle of a ZYX euler angle sequence to define initial orientation of vehicle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y angle of a ZYX euler angle sequence to define initial orientation of vehicle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x angle of a ZYX euler angle sequence to define initial orientation of vehicle </t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>velocity</t>
+  </si>
+  <si>
+    <t>attitude</t>
+  </si>
+  <si>
+    <t>accel bias</t>
+  </si>
+  <si>
+    <t>gyro bias</t>
+  </si>
+  <si>
+    <t>crumb pos</t>
+  </si>
+  <si>
+    <t>angular rate</t>
+  </si>
+  <si>
+    <t>steer angle</t>
+  </si>
+  <si>
+    <t>del_rx</t>
+  </si>
+  <si>
+    <t>del_ry</t>
+  </si>
+  <si>
+    <t>del_rz</t>
+  </si>
+  <si>
+    <t>Injected vehicle position error</t>
+  </si>
+  <si>
+    <t>del_vx</t>
+  </si>
+  <si>
+    <t>del_vy</t>
+  </si>
+  <si>
+    <t>del_vz</t>
+  </si>
+  <si>
+    <t>Injected vehicle velocity error</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>del_thetax</t>
+  </si>
+  <si>
+    <t>Injected vehicle orientation error</t>
+  </si>
+  <si>
+    <t>del_thetay</t>
+  </si>
+  <si>
+    <t>del_thetaz</t>
+  </si>
+  <si>
+    <t>del_accelx</t>
+  </si>
+  <si>
+    <t>m/s2</t>
+  </si>
+  <si>
+    <t>Injected accelerometer bias error</t>
+  </si>
+  <si>
+    <t>del_accely</t>
+  </si>
+  <si>
+    <t>del_accelz</t>
+  </si>
+  <si>
+    <t>deg/s</t>
+  </si>
+  <si>
+    <t>Injected gyroscope bias error</t>
+  </si>
+  <si>
+    <t>del_breadx</t>
+  </si>
+  <si>
+    <t>Injected breadcrumb position error</t>
+  </si>
+  <si>
+    <t>del_bready</t>
+  </si>
+  <si>
+    <t>del_breadz</t>
   </si>
 </sst>
 </file>
@@ -684,7 +549,7 @@
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,8 +565,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -714,8 +586,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -840,11 +717,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -879,9 +772,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -910,19 +801,18 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1258,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,765 +1165,453 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="64" t="s">
-        <v>142</v>
+      <c r="E1" s="62" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="65">
+      <c r="B2" s="70">
         <v>2</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="66">
-        <f t="shared" ref="E2:E10" si="0">B2</f>
+      <c r="E2" s="70">
+        <f t="shared" ref="E2:E4" si="0">B2</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="67">
+      <c r="B3" s="70">
         <v>0.25</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="68">
+      <c r="D3" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="70">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="70" t="e">
+        <f>#REF!*0.5</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="70" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="70">
+        <v>3</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="70">
+        <f>B5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67">
-        <f>B5*0.5</f>
-        <v>3404.7101009954345</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="68">
-        <f t="shared" si="0"/>
-        <v>3404.7101009954345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="B6" s="70">
+        <v>15</v>
+      </c>
+      <c r="C6" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67">
-        <f>2*PI()/SQRT(B9)*((B11+B12+2*B13)/2)^(3/2)</f>
-        <v>6809.4202019908689</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="68">
-        <f>B5</f>
-        <v>6809.4202019908689</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="69">
-        <v>3</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="68">
+      <c r="E6" s="70">
         <f>B6</f>
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="69">
-        <v>15</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="68">
-        <f>B7</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="69">
+      <c r="A7" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="70">
         <f>12*6</f>
         <v>72</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C7" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D7" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="68">
-        <f t="shared" si="0"/>
+      <c r="E7" s="70">
+        <f>B7</f>
         <v>72</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="70">
+        <v>0</v>
+      </c>
+      <c r="C8" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="70">
+        <f>B8</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="70">
-        <v>4902.8010759999997</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="68">
-        <f>B9*1000^3</f>
-        <v>4902801076000</v>
+      <c r="A9" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="70" t="e">
+        <f>#REF!/2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="70" t="e">
+        <f>B9</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="67">
-        <v>0</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="A10" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="70">
+        <v>1</v>
+      </c>
+      <c r="C10" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="68">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D10" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="70">
+        <f t="shared" ref="E10:E12" si="1">B10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="67">
-        <v>100</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="68">
-        <f>B11*1000</f>
-        <v>100000</v>
+      <c r="A11" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="70">
+        <v>0</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="67">
+      <c r="A12" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="70">
+        <v>0</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="70">
+        <v>0</v>
+      </c>
+      <c r="C13" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="70">
+        <f t="shared" ref="E13:E18" si="2">RADIANS(B13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="70">
+        <v>0</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="70">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="70">
+        <v>180</v>
+      </c>
+      <c r="C15" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="70">
+        <f t="shared" si="2"/>
+        <v>3.1415926535897931</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="70">
+        <v>0</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="70">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="70">
         <v>10</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="68">
-        <f>B12*1000</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="67">
-        <v>1737.4</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="68">
-        <f>B13*1000</f>
-        <v>1737400</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="67">
-        <v>1737.4</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="68">
-        <f>B14*1000</f>
-        <v>1737400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15" s="67">
-        <v>13.17635815</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="68">
-        <f>RADIANS(B15)/86400</f>
-        <v>2.6616994576329732E-6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="67">
-        <v>0</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="68">
-        <f>B16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="67">
-        <v>0</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="68">
-        <f>B17</f>
-        <v>0</v>
+      <c r="C17" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="70">
+        <f t="shared" si="2"/>
+        <v>0.17453292519943295</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="67">
-        <v>0</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="68">
-        <f>B18</f>
+      <c r="A18" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="70">
+        <v>0</v>
+      </c>
+      <c r="C18" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="70">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="71">
-        <f>$B$5/2</f>
-        <v>3404.7101009954345</v>
+      <c r="A19" s="70" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="70">
+        <v>0</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="68">
-        <f t="shared" ref="E19:E21" si="1">B19</f>
-        <v>3404.7101009954345</v>
+        <v>4</v>
+      </c>
+      <c r="D19" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="70">
+        <f t="shared" ref="E19" si="3">B19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="71">
-        <f>$B$5/2</f>
-        <v>3404.7101009954345</v>
-      </c>
-      <c r="C20" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="68">
-        <f t="shared" si="1"/>
-        <v>3404.7101009954345</v>
-      </c>
+      <c r="A20" s="18"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="67"/>
+      <c r="D20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="65"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="B21" s="71">
-        <f>$B$5/2</f>
-        <v>3404.7101009954345</v>
-      </c>
-      <c r="C21" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="68">
-        <f t="shared" si="1"/>
-        <v>3404.7101009954345</v>
-      </c>
+      <c r="A21" s="18"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="67"/>
+      <c r="D21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="65"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="69">
-        <v>1</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="68">
-        <f t="shared" ref="E22:E24" si="2">B22</f>
-        <v>1</v>
+      <c r="D22" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="69">
-        <v>0</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="68">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="69">
-        <v>0</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="68">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="B25" s="67">
-        <v>0</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" s="68">
-        <f t="shared" ref="E25:E30" si="3">RADIANS(B25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="B26" s="67">
-        <v>0</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="E26" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B27" s="67">
-        <v>180</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="E27" s="68">
-        <f t="shared" si="3"/>
-        <v>3.1415926535897931</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="B28" s="67">
-        <v>0</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E28" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="B29" s="67">
-        <v>10</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="E29" s="68">
-        <f t="shared" si="3"/>
-        <v>0.17453292519943295</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="B30" s="67">
-        <v>0</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E30" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="D23" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B31" s="67">
-        <v>30</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="E31" s="68">
-        <f t="shared" ref="E31:E32" si="4">B31</f>
-        <v>30</v>
-      </c>
+      <c r="A31" s="18"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="65"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" s="67">
-        <v>0</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E32" s="68">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="A32" s="18"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="65"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="B33" s="67">
-        <v>19</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="E33" s="68">
-        <f>B33/1000</f>
-        <v>1.9E-2</v>
-      </c>
+      <c r="A33" s="18"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="65"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="B34" s="67">
-        <v>7</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E34" s="68">
-        <f>B34*0.000001</f>
-        <v>6.9999999999999999E-6</v>
-      </c>
+      <c r="A34" s="18"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="65"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="B35" s="67">
-        <v>2500</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="E35" s="68">
-        <f t="shared" ref="E35:E36" si="5">B35</f>
-        <v>2500</v>
-      </c>
+      <c r="A35" s="18"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="65"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B36" s="67">
-        <v>2500</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="E36" s="68">
-        <f t="shared" si="5"/>
-        <v>2500</v>
-      </c>
+      <c r="A36" s="18"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="65"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="B37" s="69">
-        <v>5</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="E37" s="68">
-        <f>B37</f>
-        <v>5</v>
-      </c>
+      <c r="A37" s="18"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="65"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="B38" s="54">
-        <v>1</v>
-      </c>
-      <c r="C38" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="55" t="s">
-        <v>162</v>
-      </c>
-      <c r="E38" s="56">
-        <f t="shared" ref="E38:E40" si="6">B38</f>
-        <v>1</v>
-      </c>
+      <c r="A38" s="51"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="54"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="B39" s="58">
-        <v>1</v>
-      </c>
-      <c r="C39" s="59" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="59" t="s">
-        <v>163</v>
-      </c>
-      <c r="E39" s="60">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="A39" s="55"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="58"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="51" t="s">
-        <v>206</v>
-      </c>
-      <c r="B40" s="74">
-        <v>0</v>
-      </c>
-      <c r="C40" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="52" t="s">
-        <v>205</v>
-      </c>
-      <c r="E40" s="66">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="A40" s="49"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="63"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="B41" s="69">
-        <v>0</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="E41" s="68">
-        <f t="shared" ref="E41" si="7">B41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B42" s="72">
-        <v>0</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="E42" s="73">
-        <f t="shared" ref="E42" si="8">B42</f>
-        <v>0</v>
-      </c>
+      <c r="A41" s="18"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2087,7 +1665,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -2103,7 +1681,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,129 +1706,129 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="B2" s="31">
-        <v>1575.5547637675199</v>
+        <v>0</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="E2" s="32">
         <f t="shared" ref="E2:E4" si="0">B2*1000</f>
-        <v>1575554.76376752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="34">
-        <v>-178.75415266497299</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="B3" s="31">
+        <v>0</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="E3" s="32">
         <f t="shared" si="0"/>
-        <v>-178754.15266497299</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="36">
-        <v>-928.32402032916605</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="37">
+      <c r="A4" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="31">
+        <v>0</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="35">
         <f t="shared" si="0"/>
-        <v>-928324.02032916609</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="34">
-        <v>-0.50450806110878699</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>88</v>
+      <c r="A5" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="31">
+        <v>0</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="E5" s="32">
         <f>B5*1000</f>
-        <v>-504.50806110878699</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="34">
-        <v>-1.4165222911672899</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>88</v>
+      <c r="A6" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="31">
+        <v>0</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="E6" s="32">
         <f>B6*1000</f>
-        <v>-1416.5222911672899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="34">
-        <v>-0.58329957806655397</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>88</v>
+        <v>55</v>
+      </c>
+      <c r="B7" s="31">
+        <v>0</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="E7" s="32">
         <f>B7*1000</f>
-        <v>-583.29957806655398</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8" s="49">
+      <c r="A8" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="47">
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="E8" s="12">
         <f>RADIANS(B8)</f>
@@ -2258,8 +1836,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
-        <v>153</v>
+      <c r="A9" s="45" t="s">
+        <v>93</v>
       </c>
       <c r="B9" s="29">
         <v>0</v>
@@ -2268,7 +1846,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="E9" s="13">
         <f>RADIANS(B9)</f>
@@ -2276,21 +1854,21 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" s="50">
-        <v>180</v>
+      <c r="A10" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="48">
+        <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E10" s="14">
         <f>RADIANS(B10)</f>
-        <v>3.1415926535897931</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2301,39 +1879,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C720B3-BEEA-4D2E-BE7C-7EC9578AFA75}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2350,7 +1928,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -2367,7 +1945,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -2384,7 +1962,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -2393,86 +1971,130 @@
         <v>13</v>
       </c>
       <c r="D5">
+        <f>E4+1</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>D5+2</f>
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="B6">
+        <f>C5+1</f>
         <v>14</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <f>B6+0</f>
+        <v>14</v>
       </c>
       <c r="D6">
+        <f>E5+1</f>
         <v>13</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <f>D6+0</f>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="B7">
+        <f>C6+1</f>
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <f>B7+2</f>
         <v>17</v>
       </c>
-      <c r="C7">
-        <v>19</v>
-      </c>
       <c r="D7">
+        <f t="shared" ref="D7:D9" si="0">E6+1</f>
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E9" si="1">D7+2</f>
         <v>16</v>
-      </c>
-      <c r="E7">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
       <c r="B8">
-        <f>B2</f>
-        <v>1</v>
+        <f>C7+1</f>
+        <v>18</v>
       </c>
       <c r="C8">
-        <f>C4</f>
-        <v>10</v>
+        <f>B8+2</f>
+        <v>20</v>
       </c>
       <c r="D8">
-        <f>D2</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="E8">
-        <f>E4</f>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>140</v>
       </c>
       <c r="B9">
-        <f>B5</f>
-        <v>11</v>
+        <f>C8+1</f>
+        <v>21</v>
       </c>
       <c r="C9">
-        <f>C7</f>
-        <v>19</v>
+        <f>B9+2</f>
+        <v>23</v>
       </c>
       <c r="D9">
-        <f>D5</f>
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="E9">
-        <f>E7</f>
-        <v>18</v>
+      <c r="E11">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2484,35 +2106,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FD82E9-FB96-4FE4-9B12-1EDF4DE7082A}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2529,7 +2153,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -2546,7 +2170,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -2563,95 +2187,99 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="B5">
+        <f>C4+1</f>
         <v>11</v>
       </c>
       <c r="C5">
+        <f>B5+2</f>
         <v>13</v>
       </c>
       <c r="D5">
+        <f>E4+1</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f t="shared" ref="E5:E7" si="0">D5+2</f>
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="B6">
+        <f>C5+1</f>
         <v>14</v>
       </c>
       <c r="C6">
+        <f>B6+2</f>
         <v>16</v>
       </c>
       <c r="D6">
+        <f>E5+1</f>
         <v>13</v>
       </c>
       <c r="E6">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="B7">
+        <f>C6+1</f>
         <v>17</v>
       </c>
       <c r="C7">
+        <f>B7+2</f>
         <v>19</v>
       </c>
       <c r="D7">
+        <f>E6+1</f>
         <v>16</v>
       </c>
       <c r="E7">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B8">
-        <f>B2</f>
         <v>1</v>
       </c>
       <c r="C8">
-        <f>C4</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <f>D2</f>
         <v>1</v>
       </c>
       <c r="E8">
-        <f>E4</f>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9">
-        <f>B5</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <f>C7</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D9">
-        <f>D5</f>
         <v>10</v>
       </c>
       <c r="E9">
-        <f>E7</f>
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2676,35 +2304,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>142</v>
+      <c r="E1" s="40" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>159</v>
+        <v>96</v>
       </c>
       <c r="B2" s="26">
         <f>0.00000016*3</f>
         <v>4.8000000000000006E-7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>160</v>
+        <v>97</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>161</v>
+        <v>98</v>
       </c>
       <c r="E2" s="13">
         <f>B2/3</f>
@@ -2750,16 +2378,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="B5" s="10">
         <v>20</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="E5" s="13">
         <f>RADIANS(B5)/3600/3</f>
@@ -2768,16 +2396,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="B6" s="10">
         <v>20</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="E6" s="13">
         <f>RADIANS(B6)/3600/3</f>
@@ -2786,16 +2414,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="B7" s="10">
         <v>1.5</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="E7" s="13">
         <f>RADIANS(B7)/3600/3</f>
@@ -2804,16 +2432,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="B8" s="10">
         <v>1.5</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" ref="E8:E9" si="0">RADIANS(B8)/3600/3</f>
@@ -2822,16 +2450,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="B9" s="10">
         <v>9</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="0"/>
@@ -2839,17 +2467,17 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
-        <v>165</v>
+      <c r="A10" s="49" t="s">
+        <v>100</v>
       </c>
       <c r="B10" s="27">
         <v>3</v>
       </c>
-      <c r="C10" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>168</v>
+      <c r="C10" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>103</v>
       </c>
       <c r="E10" s="12">
         <f>B10/3</f>
@@ -2858,16 +2486,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>166</v>
+        <v>101</v>
       </c>
       <c r="B11" s="20">
         <v>3</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>164</v>
+        <v>99</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>167</v>
+        <v>102</v>
       </c>
       <c r="E11" s="14">
         <f>B11/3</f>
@@ -2876,7 +2504,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>184</v>
+        <v>116</v>
       </c>
       <c r="B12" s="9">
         <v>10</v>
@@ -2885,7 +2513,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>185</v>
+        <v>117</v>
       </c>
       <c r="E12" s="1">
         <f>B12/3</f>
@@ -2894,7 +2522,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>186</v>
+        <v>118</v>
       </c>
       <c r="B13" s="9">
         <v>100</v>
@@ -2903,7 +2531,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>187</v>
+        <v>119</v>
       </c>
       <c r="E13" s="1">
         <f>B13/3</f>
@@ -2912,7 +2540,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>188</v>
+        <v>120</v>
       </c>
       <c r="B14" s="9">
         <v>10</v>
@@ -2921,7 +2549,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>189</v>
+        <v>121</v>
       </c>
       <c r="E14" s="1">
         <f>B14/3</f>
@@ -2966,12 +2594,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="B2" s="4">
         <v>4000</v>
@@ -2980,7 +2608,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E2" s="12">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
@@ -2989,7 +2617,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="B3" s="6">
         <v>4000</v>
@@ -2998,7 +2626,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E3" s="13">
         <f t="shared" si="0"/>
@@ -3007,7 +2635,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="B4" s="6">
         <v>4000</v>
@@ -3016,7 +2644,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E4" s="13">
         <f t="shared" si="0"/>
@@ -3025,16 +2653,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B5" s="6">
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="0"/>
@@ -3043,16 +2671,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="B6" s="6">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="0"/>
@@ -3061,16 +2689,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="B7" s="6">
         <v>3</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="E7" s="13">
         <f t="shared" si="0"/>
@@ -3079,7 +2707,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="B8" s="6">
         <v>5.0000000000000001E-4</v>
@@ -3088,7 +2716,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" si="0"/>
@@ -3097,7 +2725,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="B9" s="6">
         <v>5.0000000000000001E-4</v>
@@ -3106,7 +2734,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="0"/>
@@ -3115,7 +2743,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B10" s="6">
         <v>5.0000000000000001E-4</v>
@@ -3124,7 +2752,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="0"/>
@@ -3133,17 +2761,17 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="B11" s="6">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="E11" s="13">
         <f>RADIANS(B11)/3600/3</f>
@@ -3152,17 +2780,17 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="B12" s="6">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="E12" s="13">
         <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
@@ -3171,17 +2799,17 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="B13" s="6">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="E13" s="13">
         <f t="shared" si="1"/>
@@ -3190,17 +2818,17 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="B14" s="6">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="E14" s="13">
         <f t="shared" si="1"/>
@@ -3209,17 +2837,17 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="B15" s="6">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="E15" s="13">
         <f t="shared" si="1"/>
@@ -3228,17 +2856,17 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="B16" s="6">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="E16" s="13">
         <f t="shared" si="1"/>
@@ -3247,7 +2875,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="B17" s="6">
         <f>truthStateParams!$B$3</f>
@@ -3257,7 +2885,7 @@
         <v>25</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="E17" s="13">
         <f>RADIANS(B17)/hr2sec/3</f>
@@ -3266,7 +2894,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B18" s="6">
         <f>truthStateParams!$B$3</f>
@@ -3276,7 +2904,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="E18" s="13">
         <f>RADIANS(B18)/hr2sec/3</f>
@@ -3285,7 +2913,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="B19" s="8">
         <f>truthStateParams!$B$3</f>
@@ -3295,7 +2923,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="E19" s="14">
         <f>RADIANS(B19)/hr2sec/3</f>
@@ -3326,20 +2954,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>142</v>
+      <c r="E1" s="40" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3523,7 +3151,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="str">
+      <c r="A10" s="49" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
       </c>
@@ -3531,11 +3159,11 @@
         <f>truthStateParams!B10</f>
         <v>3</v>
       </c>
-      <c r="C10" s="52" t="str">
+      <c r="C10" s="50" t="str">
         <f>truthStateParams!C10</f>
         <v>pixels</v>
       </c>
-      <c r="D10" s="52" t="str">
+      <c r="D10" s="50" t="str">
         <f>truthStateParams!D10</f>
         <v>3-sigma u component of pixel noise</v>
       </c>
@@ -3657,20 +3285,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3690,7 +3318,7 @@
         <f>truthStateInitialUncertainty!D2</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E2" s="43">
+      <c r="E2" s="41">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
         <v>1333.3333333333333</v>
       </c>
@@ -3713,7 +3341,7 @@
         <f>truthStateInitialUncertainty!D3</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="41">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
@@ -3736,7 +3364,7 @@
         <f>truthStateInitialUncertainty!D4</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="41">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
@@ -3759,7 +3387,7 @@
         <f>truthStateInitialUncertainty!D5</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3782,7 +3410,7 @@
         <f>truthStateInitialUncertainty!D6</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3804,7 +3432,7 @@
         <f>truthStateInitialUncertainty!D7</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3826,7 +3454,7 @@
         <f>truthStateInitialUncertainty!D8</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="41">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
@@ -3848,7 +3476,7 @@
         <f>truthStateInitialUncertainty!D9</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="41">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
@@ -3870,7 +3498,7 @@
         <f>truthStateInitialUncertainty!D10</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="41">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
@@ -3892,7 +3520,7 @@
         <f>truthStateInitialUncertainty!D11</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="41">
         <f>RADIANS(B11)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -3914,7 +3542,7 @@
         <f>truthStateInitialUncertainty!D12</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="41">
         <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -3936,7 +3564,7 @@
         <f>truthStateInitialUncertainty!D13</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="41">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -3958,7 +3586,7 @@
         <f>truthStateInitialUncertainty!D14</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="41">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -3980,7 +3608,7 @@
         <f>truthStateInitialUncertainty!D15</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="41">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -4002,7 +3630,7 @@
         <f>truthStateInitialUncertainty!D16</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="41">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -4024,7 +3652,7 @@
         <f>truthStateInitialUncertainty!D17</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="41">
         <f>RADIANS(B17)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
@@ -4046,7 +3674,7 @@
         <f>truthStateInitialUncertainty!D18</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="41">
         <f>RADIANS(B18)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
@@ -4068,7 +3696,7 @@
         <f>truthStateInitialUncertainty!D19</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E19" s="44">
+      <c r="E19" s="42">
         <f>RADIANS(B19)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
@@ -4083,389 +3711,374 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>142</v>
+      <c r="E1" s="40" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B2" s="6">
-        <v>100</v>
-      </c>
-      <c r="C2" s="6" t="str">
-        <f>truthStateInitialUncertainty!C2</f>
-        <v>m</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="43">
-        <f t="shared" ref="E2:E7" si="0">B2</f>
-        <v>100</v>
+        <v>146</v>
+      </c>
+      <c r="E2" s="41">
+        <f t="shared" ref="E2:E13" si="0">B2</f>
+        <v>0</v>
       </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="B3" s="6">
-        <v>200</v>
-      </c>
-      <c r="C3" s="6" t="str">
-        <f>truthStateInitialUncertainty!C3</f>
-        <v>m</v>
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="43">
+        <v>146</v>
+      </c>
+      <c r="E3" s="41">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="B4" s="6">
-        <v>300</v>
-      </c>
-      <c r="C4" s="6" t="str">
-        <f>truthStateInitialUncertainty!C4</f>
-        <v>m</v>
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="43">
+        <v>146</v>
+      </c>
+      <c r="E4" s="41">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6" t="str">
-        <f>truthStateInitialUncertainty!C5</f>
-        <v>m/sec</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5" s="43">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="41">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B6" s="6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="6" t="str">
-        <f>truthStateInitialUncertainty!C6</f>
-        <v>m/sec</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="43">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="41">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B7" s="6">
-        <v>3</v>
-      </c>
-      <c r="C7" s="6" t="str">
-        <f>truthStateInitialUncertainty!C7</f>
-        <v>m/sec</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E7" s="43">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="41">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8" s="43">
-        <f>B8/1000</f>
-        <v>1E-3</v>
+        <v>152</v>
+      </c>
+      <c r="B8" s="16">
+        <v>0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="41">
+        <f t="shared" ref="E8:E10" si="1">RADIANS(B8)/3600</f>
+        <v>0</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="6">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="43">
-        <f>B9/1000</f>
-        <v>2E-3</v>
+        <v>154</v>
+      </c>
+      <c r="B9" s="16">
+        <v>0</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="6">
-        <v>3</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="43">
-        <f>B10/1000</f>
-        <v>3.0000000000000001E-3</v>
+        <v>155</v>
+      </c>
+      <c r="B10" s="16">
+        <v>0</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="6">
-        <v>180</v>
-      </c>
-      <c r="C11" s="6" t="str">
-        <f>truthStateInitialUncertainty!C11</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E11" s="43">
-        <f t="shared" ref="E11:E16" si="1">RADIANS(B11)/3600</f>
-        <v>8.726646259971648E-4</v>
+        <v>156</v>
+      </c>
+      <c r="B11" s="16">
+        <v>0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="6">
-        <v>150</v>
-      </c>
-      <c r="C12" s="6" t="str">
-        <f>truthStateInitialUncertainty!C12</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E12" s="43">
-        <f t="shared" si="1"/>
-        <v>7.2722052166430398E-4</v>
+        <v>159</v>
+      </c>
+      <c r="B12" s="16">
+        <v>0</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="6">
-        <v>130</v>
-      </c>
-      <c r="C13" s="6" t="str">
-        <f>truthStateInitialUncertainty!C13</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E13" s="43">
-        <f t="shared" si="1"/>
-        <v>6.3025778544239684E-4</v>
+        <v>160</v>
+      </c>
+      <c r="B13" s="16">
+        <v>0</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14" s="6">
-        <v>180</v>
-      </c>
-      <c r="C14" s="6" t="str">
-        <f>truthStateInitialUncertainty!C14</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" s="43">
-        <f t="shared" si="1"/>
-        <v>8.726646259971648E-4</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="16">
+        <v>0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="41">
+        <f>RADIANS(B14)</f>
+        <v>0</v>
       </c>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="6">
-        <v>150</v>
-      </c>
-      <c r="C15" s="6" t="str">
-        <f>truthStateInitialUncertainty!C15</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E15" s="43">
-        <f t="shared" si="1"/>
-        <v>7.2722052166430398E-4</v>
+        <v>28</v>
+      </c>
+      <c r="B15" s="16">
+        <v>0</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" s="41">
+        <f t="shared" ref="E15:E16" si="2">RADIANS(B15)</f>
+        <v>0</v>
       </c>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="6">
-        <v>130</v>
-      </c>
-      <c r="C16" s="6" t="str">
-        <f>truthStateInitialUncertainty!C16</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="43">
-        <f t="shared" si="1"/>
-        <v>6.3025778544239684E-4</v>
+        <v>29</v>
+      </c>
+      <c r="B16" s="16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6" t="str">
-        <f>truthStateInitialUncertainty!C17</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="43">
-        <f>RADIANS(B17)/hr2sec</f>
-        <v>4.8481368110953598E-6</v>
+        <v>163</v>
+      </c>
+      <c r="B17" s="16">
+        <v>0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E17" s="41">
+        <f>B17</f>
+        <v>0</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="6">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6" t="str">
-        <f>truthStateInitialUncertainty!C18</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="43">
-        <f>RADIANS(B18)/hr2sec</f>
-        <v>4.8481368110953598E-6</v>
+        <v>165</v>
+      </c>
+      <c r="B18" s="16">
+        <v>0</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="41">
+        <f>B18</f>
+        <v>0</v>
       </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>30</v>
+        <v>166</v>
       </c>
       <c r="B19" s="8">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8" t="str">
-        <f>truthStateInitialUncertainty!C19</f>
-        <v>deg/hr</v>
+        <v>0</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="44">
-        <f>RADIANS(B19)/hr2sec</f>
-        <v>4.8481368110953598E-6</v>
+        <v>164</v>
+      </c>
+      <c r="E19" s="42">
+        <f>B19</f>
+        <v>0</v>
       </c>
       <c r="F19" s="8"/>
     </row>

</xml_diff>

<commit_message>
finished initialize_truth_state.m, working on initialize_nav_state.m
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labuser\Desktop\breadcrumb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D810ED-CAF2-4E77-82D7-E335A9D164B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331A1B29-A993-48B8-B8C6-1347ADAE8AA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="14400" windowHeight="8190" tabRatio="894" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="14400" windowHeight="8190" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="192">
   <si>
     <t>Value</t>
   </si>
@@ -452,21 +452,6 @@
     <t>attitude</t>
   </si>
   <si>
-    <t>accel bias</t>
-  </si>
-  <si>
-    <t>gyro bias</t>
-  </si>
-  <si>
-    <t>crumb pos</t>
-  </si>
-  <si>
-    <t>angular rate</t>
-  </si>
-  <si>
-    <t>steer angle</t>
-  </si>
-  <si>
     <t>del_rx</t>
   </si>
   <si>
@@ -537,6 +522,96 @@
   </si>
   <si>
     <t>del_breadz</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>angular_rate</t>
+  </si>
+  <si>
+    <t>steer_angle</t>
+  </si>
+  <si>
+    <t>accel_bias</t>
+  </si>
+  <si>
+    <t>gyro_bias</t>
+  </si>
+  <si>
+    <t>crumb_pos</t>
+  </si>
+  <si>
+    <t>angrate_x</t>
+  </si>
+  <si>
+    <t>x angluar rate of the vehicle</t>
+  </si>
+  <si>
+    <t>angrate_y</t>
+  </si>
+  <si>
+    <t>angrate_z</t>
+  </si>
+  <si>
+    <t>y angluar rate of the vehicle</t>
+  </si>
+  <si>
+    <t>z angluar rate of the vehicle</t>
+  </si>
+  <si>
+    <t>steer_ang</t>
+  </si>
+  <si>
+    <t>steering angle of the vehicle</t>
+  </si>
+  <si>
+    <t>accl_bias_x</t>
+  </si>
+  <si>
+    <t>accelerometer bias in the x direction</t>
+  </si>
+  <si>
+    <t>accl_bias_y</t>
+  </si>
+  <si>
+    <t>accl_bias_z</t>
+  </si>
+  <si>
+    <t>accelerometer bias in the y direction</t>
+  </si>
+  <si>
+    <t>accelerometer bias in the z direction</t>
+  </si>
+  <si>
+    <t>gyro_bias_x</t>
+  </si>
+  <si>
+    <t>gyro_bias_z</t>
+  </si>
+  <si>
+    <t>gyroscope bias around x</t>
+  </si>
+  <si>
+    <t>gyro_bias_y</t>
+  </si>
+  <si>
+    <t>crumb_pos_x</t>
+  </si>
+  <si>
+    <t>breadcrumb position in x</t>
+  </si>
+  <si>
+    <t>crumb_pos_y</t>
+  </si>
+  <si>
+    <t>crumb_pos_z</t>
+  </si>
+  <si>
+    <t>breadcrumb position in y</t>
+  </si>
+  <si>
+    <t>breadcrumb position in z</t>
   </si>
 </sst>
 </file>
@@ -737,10 +812,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -768,12 +842,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -782,33 +851,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1151,467 +1212,513 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D23"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="61" t="s">
+      <c r="B1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="46" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="70">
+      <c r="B2" s="47">
         <v>2</v>
       </c>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="70">
+      <c r="E2" s="47">
         <f t="shared" ref="E2:E4" si="0">B2</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="70">
+      <c r="B3" s="47">
         <v>0.25</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="70">
+      <c r="E3" s="47">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="70" t="e">
-        <f>#REF!*0.5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C4" s="70" t="s">
+      <c r="B4" s="47">
+        <v>0</v>
+      </c>
+      <c r="C4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="70" t="e">
+      <c r="E4" s="47">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="70">
+      <c r="B5" s="47">
         <v>3</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="70">
+      <c r="E5" s="47">
         <f>B5</f>
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="70">
+      <c r="B6" s="47">
         <v>15</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="47">
         <f>B6</f>
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="70">
+      <c r="B7" s="47">
         <f>12*6</f>
         <v>72</v>
       </c>
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="70">
+      <c r="E7" s="47">
         <f>B7</f>
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="70">
-        <v>0</v>
-      </c>
-      <c r="C8" s="70" t="s">
+      <c r="B8" s="47">
+        <v>0</v>
+      </c>
+      <c r="C8" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E8" s="47">
         <f>B8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="70" t="e">
-        <f>#REF!/2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="70" t="s">
+      <c r="B9" s="47">
+        <v>0</v>
+      </c>
+      <c r="C9" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="70" t="e">
+      <c r="E9" s="47">
         <f>B9</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="70">
+      <c r="B10" s="47">
         <v>1</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="70">
+      <c r="E10" s="47">
         <f t="shared" ref="E10:E12" si="1">B10</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="70">
-        <v>0</v>
-      </c>
-      <c r="C11" s="70" t="s">
+      <c r="B11" s="47">
+        <v>0</v>
+      </c>
+      <c r="C11" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="70">
+      <c r="E11" s="47">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="70">
-        <v>0</v>
-      </c>
-      <c r="C12" s="70" t="s">
+      <c r="B12" s="47">
+        <v>0</v>
+      </c>
+      <c r="C12" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="70">
+      <c r="E12" s="47">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="70">
-        <v>0</v>
-      </c>
-      <c r="C13" s="70" t="s">
+      <c r="B13" s="47">
+        <v>0</v>
+      </c>
+      <c r="C13" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="70">
+      <c r="E13" s="47">
         <f t="shared" ref="E13:E18" si="2">RADIANS(B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="70">
-        <v>0</v>
-      </c>
-      <c r="C14" s="70" t="s">
+      <c r="B14" s="47">
+        <v>0</v>
+      </c>
+      <c r="C14" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="70" t="s">
+      <c r="D14" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="70">
+      <c r="E14" s="47">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="70">
+      <c r="B15" s="47">
         <v>180</v>
       </c>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="70">
+      <c r="E15" s="47">
         <f t="shared" si="2"/>
         <v>3.1415926535897931</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="70">
-        <v>0</v>
-      </c>
-      <c r="C16" s="70" t="s">
+      <c r="B16" s="47">
+        <v>0</v>
+      </c>
+      <c r="C16" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="70">
+      <c r="E16" s="47">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="70">
+      <c r="B17" s="47">
         <v>10</v>
       </c>
-      <c r="C17" s="70" t="s">
+      <c r="C17" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="70" t="s">
+      <c r="D17" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="70">
+      <c r="E17" s="47">
         <f t="shared" si="2"/>
         <v>0.17453292519943295</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="B18" s="70">
-        <v>0</v>
-      </c>
-      <c r="C18" s="70" t="s">
+      <c r="B18" s="47">
+        <v>0</v>
+      </c>
+      <c r="C18" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="70" t="s">
+      <c r="D18" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="70">
+      <c r="E18" s="47">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="70">
-        <v>0</v>
-      </c>
-      <c r="C19" s="70" t="s">
+      <c r="B19" s="47">
+        <v>0</v>
+      </c>
+      <c r="C19" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="70" t="s">
+      <c r="D19" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="70">
-        <f t="shared" ref="E19" si="3">B19</f>
+      <c r="E19" s="47">
+        <f t="shared" ref="E19:E23" si="3">B19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="67"/>
-      <c r="D20" t="s">
+      <c r="A20" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="15">
+        <v>88</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E20" s="65"/>
+      <c r="E20" s="5">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="68"/>
-      <c r="C21" s="67"/>
-      <c r="D21" t="s">
+      <c r="A21" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="15">
+        <v>88</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E21" s="65"/>
+      <c r="E21" s="5">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="A22" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="15">
+        <v>88</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>127</v>
       </c>
+      <c r="E22" s="5">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="A23" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="15">
+        <v>88</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>128</v>
       </c>
+      <c r="E23" s="5">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="65"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="49"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="65"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="49"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="65"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="49"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="64"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="65"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="49"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="65"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="49"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="65"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="49"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="66"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="65"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="49"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="51"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="54"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="50"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="55"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="58"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="50"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="63"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="49"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="66"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="65"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1678,198 +1785,501 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="53" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="31">
-        <v>0</v>
-      </c>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="54">
+        <v>0</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="55">
         <f t="shared" ref="E2:E4" si="0">B2*1000</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="31">
-        <v>0</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="54">
+        <v>0</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="31">
-        <v>0</v>
-      </c>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="54">
+        <v>0</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="31">
-        <v>0</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="54">
+        <v>0</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="55">
         <f>B5*1000</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="31">
-        <v>0</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="54">
+        <v>0</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="55">
         <f>B6*1000</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="31">
-        <v>0</v>
-      </c>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="54">
+        <v>0</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="55">
         <f>B7*1000</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="47">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="28">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <f>RADIANS(B8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="29">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="28">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <f>RADIANS(B9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="48">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="56">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="10">
         <f>RADIANS(B10)</f>
         <v>0</v>
       </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="56">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="10">
+        <f>RADIANS(B11)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="56">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="10">
+        <f>RADIANS(B12)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="56">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" s="10">
+        <f>RADIANS(B13)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="56">
+        <v>0</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="49">
+        <f>RADIANS(B14)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" s="56">
+        <v>0</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E15" s="49">
+        <f>RADIANS(B15)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="56">
+        <v>0</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="49">
+        <f>RADIANS(B16)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="56">
+        <v>0</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17" s="49">
+        <f>RADIANS(B17)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="56">
+        <v>0</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E18" s="49">
+        <f>RADIANS(B18)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="56">
+        <v>0</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="49">
+        <f>RADIANS(B19)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" s="56">
+        <v>0</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="49">
+        <f>RADIANS(B20)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="56">
+        <v>0</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="49">
+        <f>RADIANS(B21)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="56">
+        <v>0</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="49">
+        <f>RADIANS(B22)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="56">
+        <v>0</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E23" s="49">
+        <f>RADIANS(B23)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1882,7 +2292,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,7 +2372,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -1981,7 +2391,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="B6">
         <f>C5+1</f>
@@ -2002,7 +2412,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="B7">
         <f>C6+1</f>
@@ -2023,7 +2433,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B8">
         <f>C7+1</f>
@@ -2044,7 +2454,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="B9">
         <f>C8+1</f>
@@ -2107,7 +2517,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2597,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="B5">
         <f>C4+1</f>
@@ -2208,7 +2618,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B6">
         <f>C5+1</f>
@@ -2229,7 +2639,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="B7">
         <f>C6+1</f>
@@ -2296,7 +2706,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -2304,215 +2714,215 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="34" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="25">
         <f>0.00000016*3</f>
         <v>4.8000000000000006E-7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <f>B2/3</f>
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>5</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <f>RADIANS(B3)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>0.05</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <f>RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>20</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <f>RADIANS(B5)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>20</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <f>RADIANS(B6)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>1.5</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <f>RADIANS(B7)/3600/3</f>
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>1.5</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <f t="shared" ref="E8:E9" si="0">RADIANS(B8)/3600/3</f>
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>9</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <f t="shared" si="0"/>
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="26">
         <v>3</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <f>B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <v>3</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <f>B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>10</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>117</v>
       </c>
       <c r="E12" s="1">
@@ -2521,16 +2931,16 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>100</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>119</v>
       </c>
       <c r="E13" s="1">
@@ -2539,16 +2949,16 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>10</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>121</v>
       </c>
       <c r="E14" s="1">
@@ -2572,360 +2982,360 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>4000</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
         <v>1333.3333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>4000</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>4000</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <f>RADIANS(B11)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f>truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <f>RADIANS(B17)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <f>truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <f>RADIANS(B18)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <f>truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <f>RADIANS(B19)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
@@ -2944,318 +3354,318 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="34" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="str">
+      <c r="A2" s="4" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="25">
         <f>truthStateParams!B2</f>
         <v>4.8000000000000006E-7</v>
       </c>
-      <c r="C2" s="6" t="str">
+      <c r="C2" s="5" t="str">
         <f>truthStateParams!C2</f>
         <v>m^2/s^3</v>
       </c>
-      <c r="D2" s="16" t="str">
+      <c r="D2" s="15" t="str">
         <f>truthStateParams!D2</f>
         <v>3-sigma non-gravitational process noise</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <f>B2/3</f>
         <v>1.6000000000000003E-7</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <f>truthStateParams!B3</f>
         <v>5</v>
       </c>
-      <c r="C3" s="26" t="str">
+      <c r="C3" s="25" t="str">
         <f>truthStateParams!C3</f>
         <v>deg/hr</v>
       </c>
-      <c r="D3" s="6" t="str">
+      <c r="D3" s="5" t="str">
         <f>truthStateParams!D3</f>
         <v>3-sigma steady-state gyro bias</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <f>RADIANS(B3)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="str">
+      <c r="A4" s="6" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <f>truthStateParams!B4</f>
         <v>0.05</v>
       </c>
-      <c r="C4" s="8" t="str">
+      <c r="C4" s="7" t="str">
         <f>truthStateParams!C4</f>
         <v>deg/sqrt(hr)</v>
       </c>
-      <c r="D4" s="8" t="str">
+      <c r="D4" s="7" t="str">
         <f>truthStateParams!D4</f>
         <v>3-sigma angular random walk</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <f>RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.8481368110953598E-6</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <f>truthStateParams!B5</f>
         <v>20</v>
       </c>
-      <c r="C5" s="16" t="str">
+      <c r="C5" s="15" t="str">
         <f>truthStateParams!C5</f>
         <v>arcsec/axis</v>
       </c>
-      <c r="D5" s="16" t="str">
+      <c r="D5" s="15" t="str">
         <f>truthStateParams!D5</f>
         <v>3-sigma steady-state star camera misalignment</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <f>RADIANS(B5)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <f>truthStateParams!B6</f>
         <v>20</v>
       </c>
-      <c r="C6" s="16" t="str">
+      <c r="C6" s="15" t="str">
         <f>truthStateParams!C6</f>
         <v>arcsec/axis</v>
       </c>
-      <c r="D6" s="16" t="str">
+      <c r="D6" s="15" t="str">
         <f>truthStateParams!D6</f>
         <v>3-sigma steady-state terrain camera misalignment</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <f>RADIANS(B6)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="str">
+      <c r="A7" s="17" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <f>truthStateParams!B7</f>
         <v>1.5</v>
       </c>
-      <c r="C7" s="16" t="str">
+      <c r="C7" s="15" t="str">
         <f>truthStateParams!C7</f>
         <v>arcsec</v>
       </c>
-      <c r="D7" s="16" t="str">
+      <c r="D7" s="15" t="str">
         <f>truthStateParams!D7</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <f>RADIANS(B7)/3600/3</f>
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="str">
+      <c r="A8" s="17" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <f>truthStateParams!B8</f>
         <v>1.5</v>
       </c>
-      <c r="C8" s="16" t="str">
+      <c r="C8" s="15" t="str">
         <f>truthStateParams!C8</f>
         <v>arcsec</v>
       </c>
-      <c r="D8" s="16" t="str">
+      <c r="D8" s="15" t="str">
         <f>truthStateParams!D8</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <f t="shared" ref="E8:E9" si="0">RADIANS(B8)/3600/3</f>
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="str">
+      <c r="A9" s="17" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <f>truthStateParams!B9</f>
         <v>9</v>
       </c>
-      <c r="C9" s="16" t="str">
+      <c r="C9" s="15" t="str">
         <f>truthStateParams!C9</f>
         <v>arcsec</v>
       </c>
-      <c r="D9" s="16" t="str">
+      <c r="D9" s="15" t="str">
         <f>truthStateParams!D9</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <f t="shared" si="0"/>
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="str">
+      <c r="A10" s="38" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="26">
         <f>truthStateParams!B10</f>
         <v>3</v>
       </c>
-      <c r="C10" s="50" t="str">
+      <c r="C10" s="39" t="str">
         <f>truthStateParams!C10</f>
         <v>pixels</v>
       </c>
-      <c r="D10" s="50" t="str">
+      <c r="D10" s="39" t="str">
         <f>truthStateParams!D10</f>
         <v>3-sigma u component of pixel noise</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <f>B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="str">
+      <c r="A11" s="18" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <f>truthStateParams!B11</f>
         <v>3</v>
       </c>
-      <c r="C11" s="17" t="str">
+      <c r="C11" s="16" t="str">
         <f>truthStateParams!C11</f>
         <v>pixels</v>
       </c>
-      <c r="D11" s="17" t="str">
+      <c r="D11" s="16" t="str">
         <f>truthStateParams!D11</f>
         <v>3-sigma v component of pixel noise</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <f>B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="str">
+      <c r="A12" s="18" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <f>truthStateParams!B12</f>
         <v>10</v>
       </c>
-      <c r="C12" s="17" t="str">
+      <c r="C12" s="16" t="str">
         <f>truthStateParams!C12</f>
         <v>m</v>
       </c>
-      <c r="D12" s="17" t="str">
+      <c r="D12" s="16" t="str">
         <f>truthStateParams!D12</f>
         <v>3-sigma change in inertial position measurement uncertainty</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <f>B12/3</f>
         <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="str">
+      <c r="A13" s="18" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="19">
         <f>truthStateParams!B13</f>
         <v>100</v>
       </c>
-      <c r="C13" s="17" t="str">
+      <c r="C13" s="16" t="str">
         <f>truthStateParams!C13</f>
         <v>m</v>
       </c>
-      <c r="D13" s="17" t="str">
+      <c r="D13" s="16" t="str">
         <f>truthStateParams!D13</f>
         <v>3-sigma LOSS feature location uncertainty</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <f>B13/3</f>
         <v>33.333333333333336</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="str">
+      <c r="A14" s="18" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="19">
         <f>truthStateParams!B14</f>
         <v>10</v>
       </c>
-      <c r="C14" s="17" t="str">
+      <c r="C14" s="16" t="str">
         <f>truthStateParams!C14</f>
         <v>m</v>
       </c>
-      <c r="D14" s="17" t="str">
+      <c r="D14" s="16" t="str">
         <f>truthStateParams!D14</f>
         <v>3-sigma change in lunar-referenced position measurement uncertainty</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <f>B14/3</f>
         <v>3.3333333333333335</v>
       </c>
@@ -3276,427 +3686,427 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="str">
+      <c r="A2" s="4" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <f>truthStateInitialUncertainty!B2</f>
         <v>4000</v>
       </c>
-      <c r="C2" s="6" t="str">
+      <c r="C2" s="5" t="str">
         <f>truthStateInitialUncertainty!C2</f>
         <v>m</v>
       </c>
-      <c r="D2" s="6" t="str">
+      <c r="D2" s="5" t="str">
         <f>truthStateInitialUncertainty!D2</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="35">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
         <v>1333.3333333333333</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <f>truthStateInitialUncertainty!B3</f>
         <v>4000</v>
       </c>
-      <c r="C3" s="6" t="str">
+      <c r="C3" s="5" t="str">
         <f>truthStateInitialUncertainty!C3</f>
         <v>m</v>
       </c>
-      <c r="D3" s="6" t="str">
+      <c r="D3" s="5" t="str">
         <f>truthStateInitialUncertainty!D3</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="35">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <f>truthStateInitialUncertainty!B4</f>
         <v>4000</v>
       </c>
-      <c r="C4" s="6" t="str">
+      <c r="C4" s="5" t="str">
         <f>truthStateInitialUncertainty!C4</f>
         <v>m</v>
       </c>
-      <c r="D4" s="6" t="str">
+      <c r="D4" s="5" t="str">
         <f>truthStateInitialUncertainty!D4</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="35">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <f>truthStateInitialUncertainty!B5</f>
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="str">
+      <c r="C5" s="5" t="str">
         <f>truthStateInitialUncertainty!C5</f>
         <v>m/sec</v>
       </c>
-      <c r="D5" s="6" t="str">
+      <c r="D5" s="5" t="str">
         <f>truthStateInitialUncertainty!D5</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <f>truthStateInitialUncertainty!B6</f>
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="str">
+      <c r="C6" s="5" t="str">
         <f>truthStateInitialUncertainty!C6</f>
         <v>m/sec</v>
       </c>
-      <c r="D6" s="6" t="str">
+      <c r="D6" s="5" t="str">
         <f>truthStateInitialUncertainty!D6</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="4" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <f>truthStateInitialUncertainty!B7</f>
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="str">
+      <c r="C7" s="5" t="str">
         <f>truthStateInitialUncertainty!C7</f>
         <v>m/sec</v>
       </c>
-      <c r="D7" s="6" t="str">
+      <c r="D7" s="5" t="str">
         <f>truthStateInitialUncertainty!D7</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="str">
+      <c r="A8" s="4" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <f>truthStateInitialUncertainty!B8</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C8" s="6" t="str">
+      <c r="C8" s="5" t="str">
         <f>truthStateInitialUncertainty!C8</f>
         <v>rad</v>
       </c>
-      <c r="D8" s="6" t="str">
+      <c r="D8" s="5" t="str">
         <f>truthStateInitialUncertainty!D8</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="35">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="str">
+      <c r="A9" s="4" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <f>truthStateInitialUncertainty!B9</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C9" s="6" t="str">
+      <c r="C9" s="5" t="str">
         <f>truthStateInitialUncertainty!C9</f>
         <v>rad</v>
       </c>
-      <c r="D9" s="6" t="str">
+      <c r="D9" s="5" t="str">
         <f>truthStateInitialUncertainty!D9</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="35">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="str">
+      <c r="A10" s="4" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <f>truthStateInitialUncertainty!B10</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C10" s="6" t="str">
+      <c r="C10" s="5" t="str">
         <f>truthStateInitialUncertainty!C10</f>
         <v>rad</v>
       </c>
-      <c r="D10" s="6" t="str">
+      <c r="D10" s="5" t="str">
         <f>truthStateInitialUncertainty!D10</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="35">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="str">
+      <c r="A11" s="4" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <f>truthStateInitialUncertainty!B11</f>
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="str">
+      <c r="C11" s="5" t="str">
         <f>truthStateInitialUncertainty!C11</f>
         <v>arcsec</v>
       </c>
-      <c r="D11" s="6" t="str">
+      <c r="D11" s="5" t="str">
         <f>truthStateInitialUncertainty!D11</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="35">
         <f>RADIANS(B11)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="str">
+      <c r="A12" s="4" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <f>truthStateInitialUncertainty!B12</f>
         <v>20</v>
       </c>
-      <c r="C12" s="6" t="str">
+      <c r="C12" s="5" t="str">
         <f>truthStateInitialUncertainty!C12</f>
         <v>arcsec</v>
       </c>
-      <c r="D12" s="6" t="str">
+      <c r="D12" s="5" t="str">
         <f>truthStateInitialUncertainty!D12</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="35">
         <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="str">
+      <c r="A13" s="4" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <f>truthStateInitialUncertainty!B13</f>
         <v>20</v>
       </c>
-      <c r="C13" s="6" t="str">
+      <c r="C13" s="5" t="str">
         <f>truthStateInitialUncertainty!C13</f>
         <v>arcsec</v>
       </c>
-      <c r="D13" s="6" t="str">
+      <c r="D13" s="5" t="str">
         <f>truthStateInitialUncertainty!D13</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="35">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="str">
+      <c r="A14" s="4" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f>truthStateInitialUncertainty!B14</f>
         <v>20</v>
       </c>
-      <c r="C14" s="6" t="str">
+      <c r="C14" s="5" t="str">
         <f>truthStateInitialUncertainty!C14</f>
         <v>arcsec</v>
       </c>
-      <c r="D14" s="6" t="str">
+      <c r="D14" s="5" t="str">
         <f>truthStateInitialUncertainty!D14</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E14" s="41">
+      <c r="E14" s="35">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="str">
+      <c r="A15" s="4" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <f>truthStateInitialUncertainty!B15</f>
         <v>20</v>
       </c>
-      <c r="C15" s="6" t="str">
+      <c r="C15" s="5" t="str">
         <f>truthStateInitialUncertainty!C15</f>
         <v>arcsec</v>
       </c>
-      <c r="D15" s="6" t="str">
+      <c r="D15" s="5" t="str">
         <f>truthStateInitialUncertainty!D15</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E15" s="41">
+      <c r="E15" s="35">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="str">
+      <c r="A16" s="4" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <f>truthStateInitialUncertainty!B16</f>
         <v>20</v>
       </c>
-      <c r="C16" s="6" t="str">
+      <c r="C16" s="5" t="str">
         <f>truthStateInitialUncertainty!C16</f>
         <v>arcsec</v>
       </c>
-      <c r="D16" s="6" t="str">
+      <c r="D16" s="5" t="str">
         <f>truthStateInitialUncertainty!D16</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="35">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="str">
+      <c r="A17" s="4" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f>truthStateInitialUncertainty!B17</f>
         <v>5</v>
       </c>
-      <c r="C17" s="6" t="str">
+      <c r="C17" s="5" t="str">
         <f>truthStateInitialUncertainty!C17</f>
         <v>deg/hr</v>
       </c>
-      <c r="D17" s="6" t="str">
+      <c r="D17" s="5" t="str">
         <f>truthStateInitialUncertainty!D17</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E17" s="41">
+      <c r="E17" s="35">
         <f>RADIANS(B17)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="str">
+      <c r="A18" s="4" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <f>truthStateInitialUncertainty!B18</f>
         <v>5</v>
       </c>
-      <c r="C18" s="6" t="str">
+      <c r="C18" s="5" t="str">
         <f>truthStateInitialUncertainty!C18</f>
         <v>deg/hr</v>
       </c>
-      <c r="D18" s="6" t="str">
+      <c r="D18" s="5" t="str">
         <f>truthStateInitialUncertainty!D18</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="35">
         <f>RADIANS(B18)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="str">
+      <c r="A19" s="6" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <f>truthStateInitialUncertainty!B19</f>
         <v>5</v>
       </c>
-      <c r="C19" s="8" t="str">
+      <c r="C19" s="7" t="str">
         <f>truthStateInitialUncertainty!C19</f>
         <v>deg/hr</v>
       </c>
-      <c r="D19" s="8" t="str">
+      <c r="D19" s="7" t="str">
         <f>truthStateInitialUncertainty!D19</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E19" s="42">
+      <c r="E19" s="36">
         <f>RADIANS(B19)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
@@ -3711,7 +4121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -3724,363 +4134,363 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="34" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="35">
+        <f t="shared" ref="E2:E13" si="0">B2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="35">
+        <f t="shared" ref="E8:E10" si="1">RADIANS(B8)/3600</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="35">
+        <f>RADIANS(B14)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="35">
+        <f t="shared" ref="E15:E16" si="2">RADIANS(B15)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2" s="41">
-        <f t="shared" ref="E2:E13" si="0">B2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="D17" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="35">
+        <f>B17</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E3" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D18" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="35">
+        <f>B18</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E5" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E7" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8" s="16">
-        <v>0</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E8" s="41">
-        <f t="shared" ref="E8:E10" si="1">RADIANS(B8)/3600</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="16">
-        <v>0</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E9" s="41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="16">
-        <v>0</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" s="41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" s="16">
-        <v>0</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E11" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="D19" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="16">
-        <v>0</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" s="16">
-        <v>0</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E13" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="16">
-        <v>0</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" s="41">
-        <f>RADIANS(B14)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="16">
-        <v>0</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15" s="41">
-        <f t="shared" ref="E15:E16" si="2">RADIANS(B15)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B17" s="16">
-        <v>0</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E17" s="41">
-        <f>B17</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" s="16">
-        <v>0</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E18" s="41">
-        <f>B18</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B19" s="8">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" s="42">
+      <c r="E19" s="36">
         <f>B19</f>
         <v>0</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates to config file for simrun
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labuser\Desktop\breadcrumb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331A1B29-A993-48B8-B8C6-1347ADAE8AA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C953C1C-7181-42D9-B4D8-F23DC9195056}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="14400" windowHeight="8190" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1788,7 +1788,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>